<commit_message>
add the retrofit lib files.
</commit_message>
<xml_diff>
--- a/前后台对接接口.xlsx
+++ b/前后台对接接口.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2 其他项目\8 思念公司\2 开发库\２设计　\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\download\sinian\scale\scaleFunShow\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="7380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="登录" sheetId="2" r:id="rId1"/>
@@ -552,10 +552,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>锅的型号，80KG的锅表示配方中主料的值。必须填写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>n_chuchengzhi</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -669,6 +665,10 @@
   </si>
   <si>
     <t>操作人姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锅的类型型号，80KG的锅表示配方中主料的值。必须填写</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,11 +761,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2041,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.5"/>
@@ -2671,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.5"/>
@@ -2702,7 +2702,7 @@
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>102</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -2715,7 +2715,7 @@
     <row r="4" spans="1:11">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="1" t="s">
         <v>100</v>
       </c>
@@ -2777,7 +2777,7 @@
       <c r="B10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -2789,39 +2789,39 @@
         <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>109</v>
+      <c r="C12" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2956,7 +2956,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2965,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -2976,7 +2976,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2984,7 +2984,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3029,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>107</v>
@@ -3071,102 +3071,102 @@
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="C17" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="C18" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="C19" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>